<commit_message>
b.d - błąd usuwania
</commit_message>
<xml_diff>
--- a/gui/inwentaryzacja.xlsx
+++ b/gui/inwentaryzacja.xlsx
@@ -1,70 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bandr\OneDrive\Studia\Python\Semestr II\Projekt-skaner-\gui\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0335DC1-F9C1-4F9A-B4C0-558FBFE307A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NAZWA PRODUKTU</t>
-  </si>
-  <si>
-    <t>POJEMNOŚĆ</t>
-  </si>
-  <si>
-    <t>WAGA PRODUKTU</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -82,26 +57,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,41 +456,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col width="19.33203125" customWidth="1" min="1" max="1"/>
+    <col width="17.6640625" customWidth="1" min="2" max="2"/>
+    <col width="17.109375" customWidth="1" min="3" max="3"/>
+    <col width="15.77734375" customWidth="1" min="4" max="4"/>
+    <col width="13.44140625" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>NAZWA PRODUKTU</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>POJEMNOŚĆ</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>WAGA PRODUKTU</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DATA</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E2" s="2"/>
+    <row r="2">
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>590</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wódka Soplica</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>591</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wino Fresco</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>wódka Lubelska</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>piwo Łomża</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>400</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>45812</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pierwsza zakładka - finish
</commit_message>
<xml_diff>
--- a/gui/inwentaryzacja.xlsx
+++ b/gui/inwentaryzacja.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -509,22 +509,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>590</t>
+          <t>290</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>wódka Soplica</t>
+          <t>wódka Lubelska</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>800</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>300</t>
         </is>
       </c>
       <c r="E3" s="3" t="n">
@@ -534,75 +534,25 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>591</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>wino Fresco</t>
+          <t>piwo Łomża</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>400</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>200</t>
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>45812</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>290</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>wódka Lubelska</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>800</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>300</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>45812</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>301</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>piwo Łomża</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="n">
         <v>45812</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nazwa produktu w a2
</commit_message>
<xml_diff>
--- a/gui/inwentaryzacja.xlsx
+++ b/gui/inwentaryzacja.xlsx
@@ -1,45 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bandr\OneDrive\Studia\Python\Semestr II\Projekt-skaner-\gui\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6357F97D-AFAE-4A3D-B1E1-801BDEB2F6BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DATA DODANIA DO BAZY</t>
+  </si>
+  <si>
+    <t>WAGA (BUTELKA + PŁYN)</t>
+  </si>
+  <si>
+    <t>ILOŚĆ PEŁNYCH BUTELEK</t>
+  </si>
+  <si>
+    <t>WAGA PŁYNU</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="238"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -57,87 +82,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -457,141 +422,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="19.33203125" customWidth="1" min="1" max="1"/>
-    <col width="43.109375" customWidth="1" min="2" max="2"/>
-    <col width="26.6640625" customWidth="1" min="3" max="3"/>
-    <col width="26.44140625" customWidth="1" min="4" max="4"/>
-    <col width="22.77734375" customWidth="1" min="5" max="5"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>DATA DODANIA DO BAZY</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>WAGA (BUTELKA + PŁYN)</t>
-        </is>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ILOŚĆ PEŁNYCH BUTELEK</t>
-        </is>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>WAGA PŁYNU</t>
-        </is>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="n"/>
-      <c r="E2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n"/>
-      <c r="E3" s="2" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="E4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="E5" s="2" t="n"/>
-    </row>
-    <row r="6">
-      <c r="E6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="E7" s="2" t="n"/>
-    </row>
-    <row r="8">
-      <c r="E8" s="2" t="n"/>
-    </row>
-    <row r="9">
-      <c r="E9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="E10" s="2" t="n"/>
-    </row>
-    <row r="11">
-      <c r="E11" s="2" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="E12" s="2" t="n"/>
-    </row>
-    <row r="13">
-      <c r="E13" s="2" t="n"/>
-    </row>
-    <row r="14">
-      <c r="E14" s="2" t="n"/>
-    </row>
-    <row r="15">
-      <c r="E15" s="2" t="n"/>
-    </row>
-    <row r="16">
-      <c r="E16" s="2" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>5901359000537</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1124</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
dodawanie nazwy do tabeli
</commit_message>
<xml_diff>
--- a/gui/inwentaryzacja.xlsx
+++ b/gui/inwentaryzacja.xlsx
@@ -1,45 +1,118 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaud\OneDrive\Pulpit\projekt\Projekt-skaner-\gui\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C327D82B-4BEE-4B68-A0F4-6A0AA1DC3824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DATA DODANIA DO BAZY</t>
+  </si>
+  <si>
+    <t>WAGA (BUTELKA + PŁYN)</t>
+  </si>
+  <si>
+    <t>ILOŚĆ PEŁNYCH BUTELEK</t>
+  </si>
+  <si>
+    <t>WAGA PŁYNU</t>
+  </si>
+  <si>
+    <t>PRODUKT</t>
+  </si>
+  <si>
+    <t>5901359000537</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1124</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>232323</t>
+  </si>
+  <si>
+    <t>2137</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1111111</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>esssssssssss</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="238"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,86 +131,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -457,160 +471,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col width="19.33203125" customWidth="1" min="1" max="1"/>
-    <col width="43.109375" customWidth="1" min="2" max="2"/>
-    <col width="26.6640625" customWidth="1" min="3" max="3"/>
-    <col width="26.44140625" customWidth="1" min="4" max="4"/>
-    <col width="22.77734375" customWidth="1" min="5" max="5"/>
+    <col min="1" max="1" width="19.36328125" customWidth="1"/>
+    <col min="2" max="2" width="43.08984375" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>DATA DODANIA DO BAZY</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>WAGA (BUTELKA + PŁYN)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ILOŚĆ PEŁNYCH BUTELEK</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>WAGA PŁYNU</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="n"/>
-      <c r="E2" s="2" t="n"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="n"/>
-      <c r="E3" s="2" t="n"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="n"/>
-      <c r="E4" s="2" t="n"/>
-    </row>
-    <row r="5">
-      <c r="E5" s="2" t="n"/>
-    </row>
-    <row r="6">
-      <c r="E6" s="2" t="n"/>
-    </row>
-    <row r="7">
-      <c r="E7" s="2" t="n"/>
-    </row>
-    <row r="8">
-      <c r="E8" s="2" t="n"/>
-    </row>
-    <row r="9">
-      <c r="E9" s="2" t="n"/>
-    </row>
-    <row r="10">
-      <c r="E10" s="2" t="n"/>
-    </row>
-    <row r="11">
-      <c r="E11" s="2" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="n"/>
-      <c r="E12" s="2" t="n"/>
-    </row>
-    <row r="13">
-      <c r="E13" s="2" t="n"/>
-    </row>
-    <row r="14">
-      <c r="E14" s="2" t="n"/>
-    </row>
-    <row r="15">
-      <c r="E15" s="2" t="n"/>
-    </row>
-    <row r="16">
-      <c r="E16" s="2" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>5901359000537</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="n">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2">
         <v>45812</v>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1124</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="n">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2">
+        <v>45813</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2">
         <v>45812</v>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>232323</t>
-        </is>
-      </c>
-      <c r="B19" s="4" t="n">
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
         <v>45812</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2137</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2">
+        <v>45812</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dokończona edycja i usuwanie inw
</commit_message>
<xml_diff>
--- a/gui/inwentaryzacja.xlsx
+++ b/gui/inwentaryzacja.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2136" yWindow="2112" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" state="visible" r:id="rId1"/>
@@ -462,10 +462,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -561,85 +561,87 @@
       <c r="G16" s="2" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>5901359000537</v>
-      </c>
-      <c r="B17" s="5" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="B17" s="5" t="n"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="2" t="n"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="2" t="n"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>5901359000537</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>45813</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>piwo Żywiec</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>5901359072145</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>45813</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>piwo Tyskie</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>5901359112568</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>45813</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>232323</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2137</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1212</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>1111111</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>45812</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>esssssssssss</t>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>piwo Lech Premium</t>
         </is>
       </c>
     </row>

</xml_diff>